<commit_message>
updated data file to include a 300ppi for each alias type
</commit_message>
<xml_diff>
--- a/methods/rasterize/rasterize.xlsx
+++ b/methods/rasterize/rasterize.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vasil\repositries\Darty-Ai\darty-ai-samples\methods\rasterize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E18A70B-0D4A-4E05-98E7-DFD7713502E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1514EA-BE7F-45A8-8425-4D390ED4DDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11385" yWindow="5940" windowWidth="20205" windowHeight="8670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,7 +381,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,7 +477,7 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>144</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -488,7 +488,7 @@
         <v>11</v>
       </c>
       <c r="E9">
-        <v>32</v>
+        <v>300</v>
       </c>
       <c r="F9">
         <v>50</v>

</xml_diff>